<commit_message>
Abstract methods in XlsxUtil
</commit_message>
<xml_diff>
--- a/G01_attendance.xlsx
+++ b/G01_attendance.xlsx
@@ -46,18 +46,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,12 +75,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -103,7 +94,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="true">
+    <row r="3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -118,30 +109,30 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" t="n">
         <v>1.0</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" t="n">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" t="n">
         <v>0.0</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add tests for XlsxUtilTest
</commit_message>
<xml_diff>
--- a/G01_attendance.xlsx
+++ b/G01_attendance.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CS2101 G01 Attendance Sheet</t>
   </si>
@@ -26,13 +26,16 @@
     <t>1-1</t>
   </si>
   <si>
-    <t>Aaron Tan</t>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>AARON TAN</t>
   </si>
   <si>
     <t>A0000000U</t>
   </si>
   <si>
-    <t>John Doe</t>
+    <t>JOHN DOE</t>
   </si>
   <si>
     <t>A0000001M</t>
@@ -80,7 +83,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -101,26 +104,35 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>